<commit_message>
Update section 6 Excel
</commit_message>
<xml_diff>
--- a/Section06/activities/Excel_Practice_Student.xlsx
+++ b/Section06/activities/Excel_Practice_Student.xlsx
@@ -1,41 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\CODE\savvyDAP\dap-curriculum\Section06\activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9525C6-E84E-4CF7-B9D0-6CC8A1CBB988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD771B6F-DD75-48C1-B922-06810A2F9068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17172" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{8D4C5268-695D-4616-9E91-53744754ABC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Payroll" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Loans" sheetId="2" r:id="rId2"/>
     <sheet name="Functions" sheetId="3" r:id="rId3"/>
+    <sheet name="Payroll" sheetId="1" r:id="rId4"/>
+    <sheet name="Homework Instructions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="209">
   <si>
     <t>Employee Payroll</t>
   </si>
@@ -620,6 +614,51 @@
   </si>
   <si>
     <t>XOR</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save the workbook and compare your workbook to the solution that we've provided.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the Payroll worksheet, Insert 4 columns after Hours Worked
+</t>
+  </si>
+  <si>
+    <t>Insert 4 columns after Overtime hours</t>
+  </si>
+  <si>
+    <t>Enter in a series of hours worked into the new columns</t>
+  </si>
+  <si>
+    <t>Enter in a series of Overtime hours into the new columns</t>
+  </si>
+  <si>
+    <t>Use the ABSOLUTE value sign: Add $ signs before values to fix the formula calculations and copy the calculations into all the neccesary cells
+($c$4 tells any new cells to always reference c4)</t>
+  </si>
+  <si>
+    <t>Add ABSOLUTE calculations for overtime</t>
+  </si>
+  <si>
+    <t>Color each section a different color</t>
+  </si>
+  <si>
+    <t>Do the totals for the month</t>
+  </si>
+  <si>
+    <t>Calculate a whole month’s worth of Pay totals</t>
+  </si>
+  <si>
+    <t>Put everything in borders</t>
+  </si>
+  <si>
+    <t>Decide for yourself how you would set the print area and format printing for this spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -629,7 +668,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,8 +699,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,8 +749,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -809,11 +872,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -873,13 +951,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,228 +1282,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D2CA6A-7C7B-42A2-BC97-252980B3146C}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94C76C0-2B2C-44F2-BC63-3FD054315D77}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>44669</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>3.5</v>
-      </c>
-      <c r="D6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>5.75</v>
-      </c>
-      <c r="D8">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>6.55</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>75</v>
-      </c>
-      <c r="D12">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13">
-        <v>40</v>
-      </c>
-      <c r="D13">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1514,18 +1403,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1757,13 +1646,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1900,17 +1789,17 @@
       <c r="D23" s="8"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
@@ -2139,18 +2028,18 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="F40" s="23" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="F40" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
@@ -2667,18 +2556,18 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="F64" s="24" t="s">
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="F64" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
@@ -3244,16 +3133,16 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B88" s="23"/>
-      <c r="C88" s="23"/>
-      <c r="D88" s="23"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="23"/>
-      <c r="H88" s="23"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="30"/>
+      <c r="F88" s="30"/>
+      <c r="G88" s="30"/>
+      <c r="H88" s="30"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
@@ -3475,18 +3364,18 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B103" s="23"/>
-      <c r="C103" s="23"/>
-      <c r="D103" s="23"/>
-      <c r="F103" s="23" t="s">
+      <c r="B103" s="30"/>
+      <c r="C103" s="30"/>
+      <c r="D103" s="30"/>
+      <c r="F103" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="G103" s="23"/>
-      <c r="H103" s="23"/>
-      <c r="I103" s="23"/>
+      <c r="G103" s="30"/>
+      <c r="H103" s="30"/>
+      <c r="I103" s="30"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
@@ -3703,21 +3592,21 @@
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A115" s="23" t="s">
+      <c r="A115" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="B115" s="23"/>
-      <c r="C115" s="23"/>
-      <c r="D115" s="23"/>
-      <c r="F115" s="23" t="s">
+      <c r="B115" s="30"/>
+      <c r="C115" s="30"/>
+      <c r="D115" s="30"/>
+      <c r="F115" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G115" s="23"/>
-      <c r="H115" s="23"/>
-      <c r="I115" s="23"/>
-      <c r="J115" s="23"/>
-      <c r="K115" s="23"/>
-      <c r="L115" s="23"/>
+      <c r="G115" s="30"/>
+      <c r="H115" s="30"/>
+      <c r="I115" s="30"/>
+      <c r="J115" s="30"/>
+      <c r="K115" s="30"/>
+      <c r="L115" s="30"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
@@ -3883,13 +3772,13 @@
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A127" s="23" t="s">
+      <c r="A127" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="B127" s="23"/>
-      <c r="C127" s="23"/>
-      <c r="D127" s="23"/>
-      <c r="E127" s="23"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="30"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
@@ -4021,18 +3910,18 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A138" s="23" t="s">
+      <c r="A138" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B138" s="23"/>
-      <c r="C138" s="23"/>
-      <c r="D138" s="23"/>
-      <c r="F138" s="23" t="s">
+      <c r="B138" s="30"/>
+      <c r="C138" s="30"/>
+      <c r="D138" s="30"/>
+      <c r="F138" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="G138" s="23"/>
-      <c r="H138" s="23"/>
-      <c r="I138" s="23"/>
+      <c r="G138" s="30"/>
+      <c r="H138" s="30"/>
+      <c r="I138" s="30"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
@@ -4246,23 +4135,23 @@
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A150" s="23" t="s">
+      <c r="A150" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="B150" s="23"/>
-      <c r="C150" s="23"/>
-      <c r="D150" s="23"/>
-      <c r="E150" s="23"/>
-      <c r="F150" s="23"/>
-      <c r="H150" s="23" t="s">
+      <c r="B150" s="30"/>
+      <c r="C150" s="30"/>
+      <c r="D150" s="30"/>
+      <c r="E150" s="30"/>
+      <c r="F150" s="30"/>
+      <c r="H150" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="I150" s="23"/>
-      <c r="J150" s="23"/>
-      <c r="K150" s="23"/>
-      <c r="L150" s="23"/>
-      <c r="M150" s="23"/>
-      <c r="N150" s="23"/>
+      <c r="I150" s="30"/>
+      <c r="J150" s="30"/>
+      <c r="K150" s="30"/>
+      <c r="L150" s="30"/>
+      <c r="M150" s="30"/>
+      <c r="N150" s="30"/>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
@@ -4851,14 +4740,14 @@
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B175" s="23" t="s">
+      <c r="B175" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="C175" s="23"/>
-      <c r="D175" s="23"/>
-      <c r="E175" s="23"/>
-      <c r="F175" s="23"/>
-      <c r="G175" s="23"/>
+      <c r="C175" s="30"/>
+      <c r="D175" s="30"/>
+      <c r="E175" s="30"/>
+      <c r="F175" s="30"/>
+      <c r="G175" s="30"/>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B176" s="5" t="s">
@@ -4994,16 +4883,16 @@
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B187" s="23" t="s">
+      <c r="B187" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="C187" s="23"/>
-      <c r="D187" s="23"/>
-      <c r="E187" s="23"/>
-      <c r="F187" s="23"/>
-      <c r="G187" s="23"/>
-      <c r="H187" s="23"/>
-      <c r="I187" s="23"/>
+      <c r="C187" s="30"/>
+      <c r="D187" s="30"/>
+      <c r="E187" s="30"/>
+      <c r="F187" s="30"/>
+      <c r="G187" s="30"/>
+      <c r="H187" s="30"/>
+      <c r="I187" s="30"/>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="s">
@@ -5295,15 +5184,15 @@
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A203" s="23" t="s">
+      <c r="A203" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="B203" s="23"/>
-      <c r="C203" s="23"/>
-      <c r="D203" s="23"/>
-      <c r="E203" s="23"/>
-      <c r="F203" s="23"/>
-      <c r="G203" s="23"/>
+      <c r="B203" s="30"/>
+      <c r="C203" s="30"/>
+      <c r="D203" s="30"/>
+      <c r="E203" s="30"/>
+      <c r="F203" s="30"/>
+      <c r="G203" s="30"/>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
@@ -5677,12 +5566,12 @@
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229" s="23" t="s">
+      <c r="A229" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B229" s="23"/>
-      <c r="C229" s="23"/>
-      <c r="D229" s="23"/>
+      <c r="B229" s="30"/>
+      <c r="C229" s="30"/>
+      <c r="D229" s="30"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
@@ -5804,6 +5693,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B187:I187"/>
+    <mergeCell ref="A203:G203"/>
+    <mergeCell ref="A229:D229"/>
+    <mergeCell ref="A127:E127"/>
+    <mergeCell ref="A138:D138"/>
+    <mergeCell ref="F138:I138"/>
+    <mergeCell ref="A150:F150"/>
+    <mergeCell ref="H150:N150"/>
     <mergeCell ref="A115:D115"/>
     <mergeCell ref="F115:L115"/>
     <mergeCell ref="A1:D1"/>
@@ -5817,17 +5715,350 @@
     <mergeCell ref="A88:H88"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="F103:I103"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B187:I187"/>
-    <mergeCell ref="A203:G203"/>
-    <mergeCell ref="A229:D229"/>
-    <mergeCell ref="A127:E127"/>
-    <mergeCell ref="A138:D138"/>
-    <mergeCell ref="F138:I138"/>
-    <mergeCell ref="A150:F150"/>
-    <mergeCell ref="H150:N150"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D2CA6A-7C7B-42A2-BC97-252980B3146C}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>5.75</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>6.55</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>75</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2018655-9909-4D2C-8D4C-303BEA72F8F8}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.21875" style="26" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="27">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="27">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.3">
+      <c r="A12" s="27">
+        <v>11</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
+        <v>12</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>